<commit_message>
detailed cleanup. trying to see if <500 mhz pll target can be made to work
</commit_message>
<xml_diff>
--- a/tracker/wspr_calc_direct_shift_lower_pll_range.xlsx
+++ b/tracker/wspr_calc_direct_shift_lower_pll_range.xlsx
@@ -8,8 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="pll 600" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="pll 700" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="pll 390" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="pll 600" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="pll 700" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="43">
   <si>
     <t xml:space="preserve">Note how it’s independent of the u4b frequency bin within the band.</t>
   </si>
@@ -283,11 +284,11 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -489,7 +490,7 @@
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -579,31 +580,31 @@
         <v>11</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="4" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H7" s="4" t="n">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J7" s="4" t="n">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L7" s="4" t="n">
-        <v>42</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -615,31 +616,31 @@
         <v>17</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="4" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H8" s="4" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J8" s="4" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="L8" s="4" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -648,35 +649,35 @@
       </c>
       <c r="D9" s="4" t="n">
         <f aca="false">(D8+1) * D4</f>
-        <v>624000000</v>
+        <v>390000000</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="4" t="n">
         <f aca="false">(F8+1) * D4</f>
-        <v>624000000</v>
+        <v>416000000</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="4" t="n">
         <f aca="false">(H8+1) * D4</f>
-        <v>598000000</v>
+        <v>416000000</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J9" s="4" t="n">
         <f aca="false">(J8+1) * D4</f>
-        <v>624000000</v>
+        <v>416000000</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="L9" s="4" t="n">
         <f aca="false">(L8+1) * D4</f>
-        <v>598000000</v>
+        <v>416000000</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -685,35 +686,35 @@
       </c>
       <c r="D10" s="4" t="n">
         <f aca="false">D8*D4</f>
-        <v>598000000</v>
+        <v>364000000</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F10" s="4" t="n">
         <f aca="false">F8*D4</f>
-        <v>598000000</v>
+        <v>390000000</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H10" s="4" t="n">
         <f aca="false">H8 * D4</f>
-        <v>572000000</v>
+        <v>390000000</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J10" s="4" t="n">
         <f aca="false">J8*D4</f>
-        <v>598000000</v>
+        <v>390000000</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="L10" s="4" t="n">
         <f aca="false">L8*D4</f>
-        <v>572000000</v>
+        <v>390000000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -742,49 +743,49 @@
       </c>
       <c r="D13" s="6" t="n">
         <f aca="false">MIN(1*(D4/D7)/D5, D6)</f>
-        <v>806787.878787879</v>
+        <v>1048575</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F13" s="6" t="n">
         <f aca="false">MIN(1*(D4/F7)/D5, D6)</f>
-        <v>739555.555555556</v>
+        <v>1048575</v>
       </c>
       <c r="G13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H13" s="6" t="n">
+      <c r="H13" s="7" t="n">
         <f aca="false">MIN((D4/H7)/D5, D6)</f>
-        <v>633904.761904762</v>
+        <v>986074.074074074</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J13" s="6" t="n">
+      <c r="J13" s="7" t="n">
         <f aca="false">MIN(1*(D4/J7)/D5, D6)</f>
-        <v>522039.215686275</v>
+        <v>806787.878787879</v>
       </c>
       <c r="K13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L13" s="7" t="n">
         <f aca="false">MIN(1*(D4/L7)/D5, D6)</f>
-        <v>422603.174603175</v>
+        <v>633904.761904762</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="D14" s="8" t="n">
         <f aca="false">MIN(2*(D4/D7) / D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F14" s="7" t="n">
+      <c r="F14" s="8" t="n">
         <f aca="false">MIN(2*(D4/F7)/D5, D6)</f>
         <v>1048575</v>
       </c>
@@ -800,21 +801,21 @@
       </c>
       <c r="J14" s="8" t="n">
         <f aca="false">MIN(2*(D4/J7)/D5,D6)</f>
-        <v>1044078.43137255</v>
+        <v>1048575</v>
       </c>
       <c r="K14" s="1" t="n">
         <v>2</v>
       </c>
       <c r="L14" s="6" t="n">
         <f aca="false">MIN(2*(D4/L7)/D5, D6)</f>
-        <v>845206.349206349</v>
+        <v>1048575</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D15" s="7" t="n">
+      <c r="D15" s="8" t="n">
         <f aca="false">MIN(3*(D4/D7)/D5, D6)</f>
         <v>1048575</v>
       </c>
@@ -823,26 +824,26 @@
       </c>
       <c r="F15" s="7" t="n">
         <f aca="false">MIN(3*(D6/F7)/D5, D6)</f>
-        <v>89478.4</v>
+        <v>134217.6</v>
       </c>
       <c r="G15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="H15" s="7" t="n">
+      <c r="H15" s="8" t="n">
         <f aca="false">MIN(3*(D4/H7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="I15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="J15" s="7" t="n">
+      <c r="J15" s="8" t="n">
         <f aca="false">MIN(3*(D4/J7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="K15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="L15" s="7" t="n">
+      <c r="L15" s="8" t="n">
         <f aca="false">MIN(3*(D4/L7)/D5,D6)</f>
         <v>1048575</v>
       </c>
@@ -962,6 +963,479 @@
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>26000000</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <f aca="false">12000/8192</f>
+        <v>1.46484375</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>1048575</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="4" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="4" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <f aca="false">(D8+1) * D4</f>
+        <v>624000000</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <f aca="false">(F8+1) * D4</f>
+        <v>624000000</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="4" t="n">
+        <f aca="false">(H8+1) * D4</f>
+        <v>598000000</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="4" t="n">
+        <f aca="false">(J8+1) * D4</f>
+        <v>624000000</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="4" t="n">
+        <f aca="false">(L8+1) * D4</f>
+        <v>598000000</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <f aca="false">D8*D4</f>
+        <v>598000000</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <f aca="false">F8*D4</f>
+        <v>598000000</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <f aca="false">H8 * D4</f>
+        <v>572000000</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="4" t="n">
+        <f aca="false">J8*D4</f>
+        <v>598000000</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="4" t="n">
+        <f aca="false">L8*D4</f>
+        <v>572000000</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7" t="n">
+        <f aca="false">MIN(1*(D4/D7)/D5, D6)</f>
+        <v>806787.878787879</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7" t="n">
+        <f aca="false">MIN(1*(D4/F7)/D5, D6)</f>
+        <v>739555.555555556</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="7" t="n">
+        <f aca="false">MIN((D4/H7)/D5, D6)</f>
+        <v>633904.761904762</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="7" t="n">
+        <f aca="false">MIN(1*(D4/J7)/D5, D6)</f>
+        <v>522039.215686275</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="8" t="n">
+        <f aca="false">MIN(1*(D4/L7)/D5, D6)</f>
+        <v>422603.174603175</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" s="8" t="n">
+        <f aca="false">MIN(2*(D4/D7) / D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" s="8" t="n">
+        <f aca="false">MIN(2*(D4/F7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" s="8" t="n">
+        <f aca="false">MIN(2*(D4/H7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J14" s="8" t="n">
+        <f aca="false">MIN(2*(D4/J7)/D5,D6)</f>
+        <v>1044078.43137255</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L14" s="7" t="n">
+        <f aca="false">MIN(2*(D4/L7)/D5, D6)</f>
+        <v>845206.349206349</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D15" s="8" t="n">
+        <f aca="false">MIN(3*(D4/D7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F15" s="8" t="n">
+        <f aca="false">MIN(3*(D6/F7)/D5, D6)</f>
+        <v>89478.4</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="H15" s="8" t="n">
+        <f aca="false">MIN(3*(D4/H7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J15" s="8" t="n">
+        <f aca="false">MIN(3*(D4/J7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="L15" s="8" t="n">
+        <f aca="false">MIN(3*(D4/L7)/D5,D6)</f>
+        <v>1048575</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J22" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="K32" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L32" s="10" t="n">
+        <v>96467329</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E39" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="E32:L32"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E32" r:id="rId1" display="  https://groups.io/g/QRPLabs/topic/si5351a_issues_with_frequency/96467329"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L39"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -1213,35 +1687,35 @@
       <c r="C13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D13" s="6" t="n">
+      <c r="D13" s="7" t="n">
         <f aca="false">MIN(1*(D4/D7)/D5, D6)</f>
         <v>739555.555555556</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="6" t="n">
+      <c r="F13" s="7" t="n">
         <f aca="false">MIN(1*(D4/F7)/D5, D6)</f>
         <v>633904.761904762</v>
       </c>
       <c r="G13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H13" s="7" t="n">
+      <c r="H13" s="8" t="n">
         <f aca="false">MIN((D4/H7)/D5, D6)</f>
         <v>522039.215686275</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J13" s="7" t="n">
+      <c r="J13" s="8" t="n">
         <f aca="false">MIN(1*(D4/J7)/D5, D6)</f>
         <v>467087.719298246</v>
       </c>
       <c r="K13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L13" s="7" t="n">
+      <c r="L13" s="8" t="n">
         <f aca="false">MIN(1*(D4/L7)/D5, D6)</f>
         <v>354986.666666667</v>
       </c>
@@ -1250,35 +1724,35 @@
       <c r="C14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="D14" s="8" t="n">
         <f aca="false">MIN(2*(D4/D7) / D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F14" s="7" t="n">
+      <c r="F14" s="8" t="n">
         <f aca="false">MIN(2*(D4/F7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="G14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H14" s="6" t="n">
+      <c r="H14" s="7" t="n">
         <f aca="false">MIN(2*(D4/H7)/D5, D6)</f>
         <v>1044078.43137255</v>
       </c>
       <c r="I14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="J14" s="6" t="n">
+      <c r="J14" s="7" t="n">
         <f aca="false">MIN(2*(D4/J7)/D5,D6)</f>
         <v>934175.438596491</v>
       </c>
       <c r="K14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="L14" s="6" t="n">
+      <c r="L14" s="7" t="n">
         <f aca="false">MIN(2*(D4/L7)/D5, D6)</f>
         <v>709973.333333333</v>
       </c>
@@ -1287,35 +1761,35 @@
       <c r="C15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D15" s="7" t="n">
+      <c r="D15" s="8" t="n">
         <f aca="false">MIN(3*(D4/D7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F15" s="7" t="n">
+      <c r="F15" s="8" t="n">
         <f aca="false">MIN(3*(D6/F7)/D5, D6)</f>
         <v>76695.7714285714</v>
       </c>
       <c r="G15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="H15" s="7" t="n">
+      <c r="H15" s="8" t="n">
         <f aca="false">MIN(3*(D4/H7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="I15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="J15" s="7" t="n">
+      <c r="J15" s="8" t="n">
         <f aca="false">MIN(3*(D4/J7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="K15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="L15" s="7" t="n">
+      <c r="L15" s="8" t="n">
         <f aca="false">MIN(3*(D4/L7)/D5,D6)</f>
         <v>1048575</v>
       </c>

</xml_diff>

<commit_message>
optimal denom for pll 500 (spreadsheet says good for 10/12/15/17/20M)
</commit_message>
<xml_diff>
--- a/tracker/wspr_calc_direct_shift_lower_pll_range.xlsx
+++ b/tracker/wspr_calc_direct_shift_lower_pll_range.xlsx
@@ -5,12 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="pll 390" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="pll 600" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="pll 700" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="pll 500" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="pll 416" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="pll 390" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="pll 600" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="pll 700" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="43">
   <si>
     <t xml:space="preserve">Note how it’s independent of the u4b frequency bin within the band.</t>
   </si>
@@ -284,11 +286,11 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -489,8 +491,8 @@
   </sheetPr>
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -580,31 +582,31 @@
         <v>11</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="4" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H7" s="4" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J7" s="4" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L7" s="4" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -616,31 +618,31 @@
         <v>17</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="4" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H8" s="4" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J8" s="4" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="L8" s="4" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -649,35 +651,35 @@
       </c>
       <c r="D9" s="4" t="n">
         <f aca="false">(D8+1) * D4</f>
-        <v>390000000</v>
+        <v>520000000</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="4" t="n">
         <f aca="false">(F8+1) * D4</f>
-        <v>416000000</v>
+        <v>520000000</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="4" t="n">
         <f aca="false">(H8+1) * D4</f>
-        <v>416000000</v>
+        <v>520000000</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J9" s="4" t="n">
         <f aca="false">(J8+1) * D4</f>
-        <v>416000000</v>
+        <v>520000000</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="L9" s="4" t="n">
         <f aca="false">(L8+1) * D4</f>
-        <v>416000000</v>
+        <v>520000000</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -686,35 +688,35 @@
       </c>
       <c r="D10" s="4" t="n">
         <f aca="false">D8*D4</f>
-        <v>364000000</v>
+        <v>494000000</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F10" s="4" t="n">
         <f aca="false">F8*D4</f>
-        <v>390000000</v>
+        <v>494000000</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H10" s="4" t="n">
         <f aca="false">H8 * D4</f>
-        <v>390000000</v>
+        <v>494000000</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J10" s="4" t="n">
         <f aca="false">J8*D4</f>
-        <v>390000000</v>
+        <v>494000000</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="L10" s="4" t="n">
         <f aca="false">L8*D4</f>
-        <v>390000000</v>
+        <v>494000000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -743,107 +745,107 @@
       </c>
       <c r="D13" s="6" t="n">
         <f aca="false">MIN(1*(D4/D7)/D5, D6)</f>
-        <v>1048575</v>
+        <v>986074.074074074</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F13" s="6" t="n">
         <f aca="false">MIN(1*(D4/F7)/D5, D6)</f>
-        <v>1048575</v>
+        <v>887466.666666667</v>
       </c>
       <c r="G13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H13" s="7" t="n">
+      <c r="H13" s="6" t="n">
         <f aca="false">MIN((D4/H7)/D5, D6)</f>
-        <v>986074.074074074</v>
+        <v>739555.555555556</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J13" s="7" t="n">
+      <c r="J13" s="6" t="n">
         <f aca="false">MIN(1*(D4/J7)/D5, D6)</f>
-        <v>806787.878787879</v>
+        <v>633904.761904762</v>
       </c>
       <c r="K13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L13" s="7" t="n">
+      <c r="L13" s="6" t="n">
         <f aca="false">MIN(1*(D4/L7)/D5, D6)</f>
-        <v>633904.761904762</v>
+        <v>493037.037037037</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D14" s="8" t="n">
+      <c r="D14" s="7" t="n">
         <f aca="false">MIN(2*(D4/D7) / D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F14" s="8" t="n">
+      <c r="F14" s="7" t="n">
         <f aca="false">MIN(2*(D4/F7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="G14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H14" s="8" t="n">
+      <c r="H14" s="7" t="n">
         <f aca="false">MIN(2*(D4/H7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="I14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="J14" s="8" t="n">
+      <c r="J14" s="7" t="n">
         <f aca="false">MIN(2*(D4/J7)/D5,D6)</f>
         <v>1048575</v>
       </c>
       <c r="K14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="L14" s="6" t="n">
+      <c r="L14" s="8" t="n">
         <f aca="false">MIN(2*(D4/L7)/D5, D6)</f>
-        <v>1048575</v>
+        <v>986074.074074074</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D15" s="8" t="n">
+      <c r="D15" s="7" t="n">
         <f aca="false">MIN(3*(D4/D7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F15" s="7" t="n">
+      <c r="F15" s="8" t="n">
         <f aca="false">MIN(3*(D6/F7)/D5, D6)</f>
-        <v>134217.6</v>
+        <v>107374.08</v>
       </c>
       <c r="G15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="H15" s="8" t="n">
+      <c r="H15" s="7" t="n">
         <f aca="false">MIN(3*(D4/H7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="I15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="J15" s="8" t="n">
+      <c r="J15" s="7" t="n">
         <f aca="false">MIN(3*(D4/J7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="K15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="L15" s="8" t="n">
+      <c r="L15" s="7" t="n">
         <f aca="false">MIN(3*(D4/L7)/D5,D6)</f>
         <v>1048575</v>
       </c>
@@ -963,7 +965,7 @@
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1053,31 +1055,31 @@
         <v>11</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="4" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H7" s="4" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J7" s="4" t="n">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L7" s="4" t="n">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1089,31 +1091,31 @@
         <v>17</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="4" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H8" s="4" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J8" s="4" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="L8" s="4" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1122,35 +1124,35 @@
       </c>
       <c r="D9" s="4" t="n">
         <f aca="false">(D8+1) * D4</f>
-        <v>624000000</v>
+        <v>416000000</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="4" t="n">
         <f aca="false">(F8+1) * D4</f>
-        <v>624000000</v>
+        <v>416000000</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="4" t="n">
         <f aca="false">(H8+1) * D4</f>
-        <v>598000000</v>
+        <v>442000000</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J9" s="4" t="n">
         <f aca="false">(J8+1) * D4</f>
-        <v>624000000</v>
+        <v>416000000</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="L9" s="4" t="n">
         <f aca="false">(L8+1) * D4</f>
-        <v>598000000</v>
+        <v>442000000</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1159,35 +1161,35 @@
       </c>
       <c r="D10" s="4" t="n">
         <f aca="false">D8*D4</f>
-        <v>598000000</v>
+        <v>390000000</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F10" s="4" t="n">
         <f aca="false">F8*D4</f>
-        <v>598000000</v>
+        <v>390000000</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H10" s="4" t="n">
         <f aca="false">H8 * D4</f>
-        <v>572000000</v>
+        <v>416000000</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J10" s="4" t="n">
         <f aca="false">J8*D4</f>
-        <v>598000000</v>
+        <v>390000000</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="L10" s="4" t="n">
         <f aca="false">L8*D4</f>
-        <v>572000000</v>
+        <v>416000000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1214,109 +1216,109 @@
       <c r="C13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D13" s="7" t="n">
+      <c r="D13" s="8" t="n">
         <f aca="false">MIN(1*(D4/D7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="8" t="n">
+        <f aca="false">MIN(1*(D4/F7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="6" t="n">
+        <f aca="false">MIN((D4/H7)/D5, D6)</f>
+        <v>887466.666666667</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="6" t="n">
+        <f aca="false">MIN(1*(D4/J7)/D5, D6)</f>
         <v>806787.878787879</v>
       </c>
-      <c r="E13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="7" t="n">
-        <f aca="false">MIN(1*(D4/F7)/D5, D6)</f>
-        <v>739555.555555556</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="7" t="n">
-        <f aca="false">MIN((D4/H7)/D5, D6)</f>
-        <v>633904.761904762</v>
-      </c>
-      <c r="I13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J13" s="7" t="n">
-        <f aca="false">MIN(1*(D4/J7)/D5, D6)</f>
-        <v>522039.215686275</v>
-      </c>
       <c r="K13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L13" s="8" t="n">
+      <c r="L13" s="6" t="n">
         <f aca="false">MIN(1*(D4/L7)/D5, D6)</f>
-        <v>422603.174603175</v>
+        <v>591644.444444444</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D14" s="8" t="n">
+      <c r="D14" s="7" t="n">
         <f aca="false">MIN(2*(D4/D7) / D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F14" s="8" t="n">
+      <c r="F14" s="7" t="n">
         <f aca="false">MIN(2*(D4/F7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="G14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H14" s="8" t="n">
+      <c r="H14" s="7" t="n">
         <f aca="false">MIN(2*(D4/H7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="I14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="J14" s="8" t="n">
+      <c r="J14" s="7" t="n">
         <f aca="false">MIN(2*(D4/J7)/D5,D6)</f>
-        <v>1044078.43137255</v>
+        <v>1048575</v>
       </c>
       <c r="K14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="L14" s="7" t="n">
+      <c r="L14" s="8" t="n">
         <f aca="false">MIN(2*(D4/L7)/D5, D6)</f>
-        <v>845206.349206349</v>
+        <v>1048575</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D15" s="8" t="n">
+      <c r="D15" s="7" t="n">
         <f aca="false">MIN(3*(D4/D7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F15" s="8" t="n">
+      <c r="F15" s="6" t="n">
         <f aca="false">MIN(3*(D6/F7)/D5, D6)</f>
-        <v>89478.4</v>
+        <v>134217.6</v>
       </c>
       <c r="G15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="H15" s="8" t="n">
+      <c r="H15" s="7" t="n">
         <f aca="false">MIN(3*(D4/H7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="I15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="J15" s="8" t="n">
+      <c r="J15" s="7" t="n">
         <f aca="false">MIN(3*(D4/J7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="K15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="L15" s="8" t="n">
+      <c r="L15" s="7" t="n">
         <f aca="false">MIN(3*(D4/L7)/D5,D6)</f>
         <v>1048575</v>
       </c>
@@ -1436,6 +1438,952 @@
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>26000000</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <f aca="false">12000/8192</f>
+        <v>1.46484375</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>1048575</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="4" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="4" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <f aca="false">(D8+1) * D4</f>
+        <v>390000000</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <f aca="false">(F8+1) * D4</f>
+        <v>416000000</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="4" t="n">
+        <f aca="false">(H8+1) * D4</f>
+        <v>416000000</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="4" t="n">
+        <f aca="false">(J8+1) * D4</f>
+        <v>416000000</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="4" t="n">
+        <f aca="false">(L8+1) * D4</f>
+        <v>416000000</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <f aca="false">D8*D4</f>
+        <v>364000000</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <f aca="false">F8*D4</f>
+        <v>390000000</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <f aca="false">H8 * D4</f>
+        <v>390000000</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="4" t="n">
+        <f aca="false">J8*D4</f>
+        <v>390000000</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="4" t="n">
+        <f aca="false">L8*D4</f>
+        <v>390000000</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="8" t="n">
+        <f aca="false">MIN(1*(D4/D7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="8" t="n">
+        <f aca="false">MIN(1*(D4/F7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="6" t="n">
+        <f aca="false">MIN((D4/H7)/D5, D6)</f>
+        <v>986074.074074074</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="6" t="n">
+        <f aca="false">MIN(1*(D4/J7)/D5, D6)</f>
+        <v>806787.878787879</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="6" t="n">
+        <f aca="false">MIN(1*(D4/L7)/D5, D6)</f>
+        <v>633904.761904762</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" s="7" t="n">
+        <f aca="false">MIN(2*(D4/D7) / D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" s="7" t="n">
+        <f aca="false">MIN(2*(D4/F7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" s="7" t="n">
+        <f aca="false">MIN(2*(D4/H7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J14" s="7" t="n">
+        <f aca="false">MIN(2*(D4/J7)/D5,D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L14" s="8" t="n">
+        <f aca="false">MIN(2*(D4/L7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D15" s="7" t="n">
+        <f aca="false">MIN(3*(D4/D7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F15" s="6" t="n">
+        <f aca="false">MIN(3*(D6/F7)/D5, D6)</f>
+        <v>134217.6</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="H15" s="7" t="n">
+        <f aca="false">MIN(3*(D4/H7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J15" s="7" t="n">
+        <f aca="false">MIN(3*(D4/J7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="L15" s="7" t="n">
+        <f aca="false">MIN(3*(D4/L7)/D5,D6)</f>
+        <v>1048575</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J22" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="K32" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L32" s="10" t="n">
+        <v>96467329</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E39" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="E32:L32"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E32" r:id="rId1" display="  https://groups.io/g/QRPLabs/topic/si5351a_issues_with_frequency/96467329"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L39"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>26000000</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <f aca="false">12000/8192</f>
+        <v>1.46484375</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>1048575</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="4" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="4" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <f aca="false">(D8+1) * D4</f>
+        <v>624000000</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <f aca="false">(F8+1) * D4</f>
+        <v>624000000</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="4" t="n">
+        <f aca="false">(H8+1) * D4</f>
+        <v>598000000</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="4" t="n">
+        <f aca="false">(J8+1) * D4</f>
+        <v>624000000</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="4" t="n">
+        <f aca="false">(L8+1) * D4</f>
+        <v>598000000</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <f aca="false">D8*D4</f>
+        <v>598000000</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <f aca="false">F8*D4</f>
+        <v>598000000</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <f aca="false">H8 * D4</f>
+        <v>572000000</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="4" t="n">
+        <f aca="false">J8*D4</f>
+        <v>598000000</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="4" t="n">
+        <f aca="false">L8*D4</f>
+        <v>572000000</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6" t="n">
+        <f aca="false">MIN(1*(D4/D7)/D5, D6)</f>
+        <v>806787.878787879</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="6" t="n">
+        <f aca="false">MIN(1*(D4/F7)/D5, D6)</f>
+        <v>739555.555555556</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="6" t="n">
+        <f aca="false">MIN((D4/H7)/D5, D6)</f>
+        <v>633904.761904762</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="6" t="n">
+        <f aca="false">MIN(1*(D4/J7)/D5, D6)</f>
+        <v>522039.215686275</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="7" t="n">
+        <f aca="false">MIN(1*(D4/L7)/D5, D6)</f>
+        <v>422603.174603175</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" s="7" t="n">
+        <f aca="false">MIN(2*(D4/D7) / D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" s="7" t="n">
+        <f aca="false">MIN(2*(D4/F7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" s="7" t="n">
+        <f aca="false">MIN(2*(D4/H7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J14" s="7" t="n">
+        <f aca="false">MIN(2*(D4/J7)/D5,D6)</f>
+        <v>1044078.43137255</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L14" s="6" t="n">
+        <f aca="false">MIN(2*(D4/L7)/D5, D6)</f>
+        <v>845206.349206349</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D15" s="7" t="n">
+        <f aca="false">MIN(3*(D4/D7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F15" s="7" t="n">
+        <f aca="false">MIN(3*(D6/F7)/D5, D6)</f>
+        <v>89478.4</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="H15" s="7" t="n">
+        <f aca="false">MIN(3*(D4/H7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J15" s="7" t="n">
+        <f aca="false">MIN(3*(D4/J7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="L15" s="7" t="n">
+        <f aca="false">MIN(3*(D4/L7)/D5,D6)</f>
+        <v>1048575</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J22" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="K32" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L32" s="10" t="n">
+        <v>96467329</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E39" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="E32:L32"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E32" r:id="rId1" display="  https://groups.io/g/QRPLabs/topic/si5351a_issues_with_frequency/96467329"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L39"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -1687,35 +2635,35 @@
       <c r="C13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D13" s="7" t="n">
+      <c r="D13" s="6" t="n">
         <f aca="false">MIN(1*(D4/D7)/D5, D6)</f>
         <v>739555.555555556</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="7" t="n">
+      <c r="F13" s="6" t="n">
         <f aca="false">MIN(1*(D4/F7)/D5, D6)</f>
         <v>633904.761904762</v>
       </c>
       <c r="G13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H13" s="8" t="n">
+      <c r="H13" s="7" t="n">
         <f aca="false">MIN((D4/H7)/D5, D6)</f>
         <v>522039.215686275</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J13" s="8" t="n">
+      <c r="J13" s="7" t="n">
         <f aca="false">MIN(1*(D4/J7)/D5, D6)</f>
         <v>467087.719298246</v>
       </c>
       <c r="K13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L13" s="8" t="n">
+      <c r="L13" s="7" t="n">
         <f aca="false">MIN(1*(D4/L7)/D5, D6)</f>
         <v>354986.666666667</v>
       </c>
@@ -1724,35 +2672,35 @@
       <c r="C14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D14" s="8" t="n">
+      <c r="D14" s="7" t="n">
         <f aca="false">MIN(2*(D4/D7) / D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F14" s="8" t="n">
+      <c r="F14" s="7" t="n">
         <f aca="false">MIN(2*(D4/F7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="G14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H14" s="7" t="n">
+      <c r="H14" s="6" t="n">
         <f aca="false">MIN(2*(D4/H7)/D5, D6)</f>
         <v>1044078.43137255</v>
       </c>
       <c r="I14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="J14" s="7" t="n">
+      <c r="J14" s="6" t="n">
         <f aca="false">MIN(2*(D4/J7)/D5,D6)</f>
         <v>934175.438596491</v>
       </c>
       <c r="K14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="L14" s="7" t="n">
+      <c r="L14" s="6" t="n">
         <f aca="false">MIN(2*(D4/L7)/D5, D6)</f>
         <v>709973.333333333</v>
       </c>
@@ -1761,35 +2709,35 @@
       <c r="C15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D15" s="8" t="n">
+      <c r="D15" s="7" t="n">
         <f aca="false">MIN(3*(D4/D7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F15" s="8" t="n">
+      <c r="F15" s="7" t="n">
         <f aca="false">MIN(3*(D6/F7)/D5, D6)</f>
         <v>76695.7714285714</v>
       </c>
       <c r="G15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="H15" s="8" t="n">
+      <c r="H15" s="7" t="n">
         <f aca="false">MIN(3*(D4/H7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="I15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="J15" s="8" t="n">
+      <c r="J15" s="7" t="n">
         <f aca="false">MIN(3*(D4/J7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="K15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="L15" s="8" t="n">
+      <c r="L15" s="7" t="n">
         <f aca="false">MIN(3*(D4/L7)/D5,D6)</f>
         <v>1048575</v>
       </c>

</xml_diff>

<commit_message>
hmm seems like PLL 500Mhz is the lowest I can go and cover 10M for optimal denom unless I shift to hans denominator-shift method
</commit_message>
<xml_diff>
--- a/tracker/wspr_calc_direct_shift_lower_pll_range.xlsx
+++ b/tracker/wspr_calc_direct_shift_lower_pll_range.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="pll 500" sheetId="1" state="visible" r:id="rId3"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="44">
   <si>
     <t xml:space="preserve">Note how it’s independent of the u4b frequency bin within the band.</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t xml:space="preserve">pll freq min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out freq max</t>
   </si>
   <si>
     <t xml:space="preserve">denom for num step</t>
@@ -261,7 +264,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -282,7 +285,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -491,8 +498,8 @@
   </sheetPr>
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M18" activeCellId="0" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -720,58 +727,92 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G11" s="5"/>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <f aca="false">D9/D7</f>
+        <v>28888888.8888889</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <f aca="false">F9/F7</f>
+        <v>26000000</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="5" t="n">
+        <f aca="false">H9/H7</f>
+        <v>21666666.6666667</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="5" t="n">
+        <f aca="false">J9/J7</f>
+        <v>18571428.5714286</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="5" t="n">
+        <f aca="false">L9/L7</f>
+        <v>14444444.4444444</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>24</v>
+      <c r="C12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D13" s="6" t="n">
+      <c r="D13" s="7" t="n">
         <f aca="false">MIN(1*(D4/D7)/D5, D6)</f>
         <v>986074.074074074</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="6" t="n">
+      <c r="F13" s="7" t="n">
         <f aca="false">MIN(1*(D4/F7)/D5, D6)</f>
         <v>887466.666666667</v>
       </c>
       <c r="G13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H13" s="6" t="n">
+      <c r="H13" s="7" t="n">
         <f aca="false">MIN((D4/H7)/D5, D6)</f>
         <v>739555.555555556</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J13" s="6" t="n">
+      <c r="J13" s="7" t="n">
         <f aca="false">MIN(1*(D4/J7)/D5, D6)</f>
         <v>633904.761904762</v>
       </c>
       <c r="K13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L13" s="6" t="n">
+      <c r="L13" s="8" t="n">
         <f aca="false">MIN(1*(D4/L7)/D5, D6)</f>
         <v>493037.037037037</v>
       </c>
@@ -780,35 +821,35 @@
       <c r="C14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="D14" s="9" t="n">
         <f aca="false">MIN(2*(D4/D7) / D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F14" s="7" t="n">
+      <c r="F14" s="9" t="n">
         <f aca="false">MIN(2*(D4/F7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="G14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H14" s="7" t="n">
+      <c r="H14" s="9" t="n">
         <f aca="false">MIN(2*(D4/H7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="I14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="J14" s="7" t="n">
+      <c r="J14" s="9" t="n">
         <f aca="false">MIN(2*(D4/J7)/D5,D6)</f>
         <v>1048575</v>
       </c>
       <c r="K14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="L14" s="8" t="n">
+      <c r="L14" s="7" t="n">
         <f aca="false">MIN(2*(D4/L7)/D5, D6)</f>
         <v>986074.074074074</v>
       </c>
@@ -817,7 +858,7 @@
       <c r="C15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D15" s="7" t="n">
+      <c r="D15" s="9" t="n">
         <f aca="false">MIN(3*(D4/D7)/D5, D6)</f>
         <v>1048575</v>
       </c>
@@ -831,105 +872,105 @@
       <c r="G15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="H15" s="7" t="n">
+      <c r="H15" s="9" t="n">
         <f aca="false">MIN(3*(D4/H7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="I15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="J15" s="7" t="n">
+      <c r="J15" s="9" t="n">
         <f aca="false">MIN(3*(D4/J7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="K15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="L15" s="7" t="n">
+      <c r="L15" s="9" t="n">
         <f aca="false">MIN(3*(D4/L7)/D5,D6)</f>
         <v>1048575</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J22" s="9" t="s">
-        <v>26</v>
+      <c r="J22" s="10" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E29" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E30" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D32" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E32" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10" t="s">
+      <c r="E32" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H32" s="10" t="s">
+      <c r="F32" s="11"/>
+      <c r="G32" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I32" s="10" t="s">
+      <c r="H32" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J32" s="10" t="s">
+      <c r="I32" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="K32" s="10" t="s">
+      <c r="J32" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="L32" s="10" t="n">
+      <c r="K32" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L32" s="11" t="n">
         <v>96467329</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E33" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E34" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E35" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E37" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E38" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E39" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1193,23 +1234,23 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G11" s="5"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>24</v>
+      <c r="C12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1230,21 +1271,21 @@
       <c r="G13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H13" s="6" t="n">
+      <c r="H13" s="7" t="n">
         <f aca="false">MIN((D4/H7)/D5, D6)</f>
         <v>887466.666666667</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J13" s="6" t="n">
+      <c r="J13" s="7" t="n">
         <f aca="false">MIN(1*(D4/J7)/D5, D6)</f>
         <v>806787.878787879</v>
       </c>
       <c r="K13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L13" s="6" t="n">
+      <c r="L13" s="7" t="n">
         <f aca="false">MIN(1*(D4/L7)/D5, D6)</f>
         <v>591644.444444444</v>
       </c>
@@ -1253,28 +1294,28 @@
       <c r="C14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="D14" s="9" t="n">
         <f aca="false">MIN(2*(D4/D7) / D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F14" s="7" t="n">
+      <c r="F14" s="9" t="n">
         <f aca="false">MIN(2*(D4/F7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="G14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H14" s="7" t="n">
+      <c r="H14" s="9" t="n">
         <f aca="false">MIN(2*(D4/H7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="I14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="J14" s="7" t="n">
+      <c r="J14" s="9" t="n">
         <f aca="false">MIN(2*(D4/J7)/D5,D6)</f>
         <v>1048575</v>
       </c>
@@ -1290,119 +1331,119 @@
       <c r="C15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D15" s="7" t="n">
+      <c r="D15" s="9" t="n">
         <f aca="false">MIN(3*(D4/D7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F15" s="6" t="n">
+      <c r="F15" s="7" t="n">
         <f aca="false">MIN(3*(D6/F7)/D5, D6)</f>
         <v>134217.6</v>
       </c>
       <c r="G15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="H15" s="7" t="n">
+      <c r="H15" s="9" t="n">
         <f aca="false">MIN(3*(D4/H7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="I15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="J15" s="7" t="n">
+      <c r="J15" s="9" t="n">
         <f aca="false">MIN(3*(D4/J7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="K15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="L15" s="7" t="n">
+      <c r="L15" s="9" t="n">
         <f aca="false">MIN(3*(D4/L7)/D5,D6)</f>
         <v>1048575</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J22" s="9" t="s">
-        <v>26</v>
+      <c r="J22" s="10" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E29" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E30" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D32" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E32" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10" t="s">
+      <c r="E32" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H32" s="10" t="s">
+      <c r="F32" s="11"/>
+      <c r="G32" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I32" s="10" t="s">
+      <c r="H32" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J32" s="10" t="s">
+      <c r="I32" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="K32" s="10" t="s">
+      <c r="J32" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="L32" s="10" t="n">
+      <c r="K32" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L32" s="11" t="n">
         <v>96467329</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E33" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E34" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E35" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E37" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E38" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E39" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1666,23 +1707,23 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G11" s="5"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>24</v>
+      <c r="C12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1703,21 +1744,21 @@
       <c r="G13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H13" s="6" t="n">
+      <c r="H13" s="7" t="n">
         <f aca="false">MIN((D4/H7)/D5, D6)</f>
         <v>986074.074074074</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J13" s="6" t="n">
+      <c r="J13" s="7" t="n">
         <f aca="false">MIN(1*(D4/J7)/D5, D6)</f>
         <v>806787.878787879</v>
       </c>
       <c r="K13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L13" s="6" t="n">
+      <c r="L13" s="7" t="n">
         <f aca="false">MIN(1*(D4/L7)/D5, D6)</f>
         <v>633904.761904762</v>
       </c>
@@ -1726,28 +1767,28 @@
       <c r="C14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="D14" s="9" t="n">
         <f aca="false">MIN(2*(D4/D7) / D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F14" s="7" t="n">
+      <c r="F14" s="9" t="n">
         <f aca="false">MIN(2*(D4/F7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="G14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H14" s="7" t="n">
+      <c r="H14" s="9" t="n">
         <f aca="false">MIN(2*(D4/H7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="I14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="J14" s="7" t="n">
+      <c r="J14" s="9" t="n">
         <f aca="false">MIN(2*(D4/J7)/D5,D6)</f>
         <v>1048575</v>
       </c>
@@ -1763,119 +1804,119 @@
       <c r="C15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D15" s="7" t="n">
+      <c r="D15" s="9" t="n">
         <f aca="false">MIN(3*(D4/D7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F15" s="6" t="n">
+      <c r="F15" s="7" t="n">
         <f aca="false">MIN(3*(D6/F7)/D5, D6)</f>
         <v>134217.6</v>
       </c>
       <c r="G15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="H15" s="7" t="n">
+      <c r="H15" s="9" t="n">
         <f aca="false">MIN(3*(D4/H7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="I15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="J15" s="7" t="n">
+      <c r="J15" s="9" t="n">
         <f aca="false">MIN(3*(D4/J7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="K15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="L15" s="7" t="n">
+      <c r="L15" s="9" t="n">
         <f aca="false">MIN(3*(D4/L7)/D5,D6)</f>
         <v>1048575</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J22" s="9" t="s">
-        <v>26</v>
+      <c r="J22" s="10" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E29" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E30" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D32" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E32" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10" t="s">
+      <c r="E32" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H32" s="10" t="s">
+      <c r="F32" s="11"/>
+      <c r="G32" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I32" s="10" t="s">
+      <c r="H32" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J32" s="10" t="s">
+      <c r="I32" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="K32" s="10" t="s">
+      <c r="J32" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="L32" s="10" t="n">
+      <c r="K32" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L32" s="11" t="n">
         <v>96467329</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E33" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E34" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E35" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E37" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E38" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E39" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1910,7 +1951,7 @@
   </sheetPr>
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -2139,58 +2180,58 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G11" s="5"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>24</v>
+      <c r="C12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D13" s="6" t="n">
+      <c r="D13" s="7" t="n">
         <f aca="false">MIN(1*(D4/D7)/D5, D6)</f>
         <v>806787.878787879</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="6" t="n">
+      <c r="F13" s="7" t="n">
         <f aca="false">MIN(1*(D4/F7)/D5, D6)</f>
         <v>739555.555555556</v>
       </c>
       <c r="G13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H13" s="6" t="n">
+      <c r="H13" s="7" t="n">
         <f aca="false">MIN((D4/H7)/D5, D6)</f>
         <v>633904.761904762</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J13" s="6" t="n">
+      <c r="J13" s="7" t="n">
         <f aca="false">MIN(1*(D4/J7)/D5, D6)</f>
         <v>522039.215686275</v>
       </c>
       <c r="K13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L13" s="7" t="n">
+      <c r="L13" s="9" t="n">
         <f aca="false">MIN(1*(D4/L7)/D5, D6)</f>
         <v>422603.174603175</v>
       </c>
@@ -2199,35 +2240,35 @@
       <c r="C14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="D14" s="9" t="n">
         <f aca="false">MIN(2*(D4/D7) / D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F14" s="7" t="n">
+      <c r="F14" s="9" t="n">
         <f aca="false">MIN(2*(D4/F7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="G14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H14" s="7" t="n">
+      <c r="H14" s="9" t="n">
         <f aca="false">MIN(2*(D4/H7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="I14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="J14" s="7" t="n">
+      <c r="J14" s="9" t="n">
         <f aca="false">MIN(2*(D4/J7)/D5,D6)</f>
         <v>1044078.43137255</v>
       </c>
       <c r="K14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="L14" s="6" t="n">
+      <c r="L14" s="7" t="n">
         <f aca="false">MIN(2*(D4/L7)/D5, D6)</f>
         <v>845206.349206349</v>
       </c>
@@ -2236,119 +2277,119 @@
       <c r="C15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D15" s="7" t="n">
+      <c r="D15" s="9" t="n">
         <f aca="false">MIN(3*(D4/D7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F15" s="7" t="n">
+      <c r="F15" s="9" t="n">
         <f aca="false">MIN(3*(D6/F7)/D5, D6)</f>
         <v>89478.4</v>
       </c>
       <c r="G15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="H15" s="7" t="n">
+      <c r="H15" s="9" t="n">
         <f aca="false">MIN(3*(D4/H7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="I15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="J15" s="7" t="n">
+      <c r="J15" s="9" t="n">
         <f aca="false">MIN(3*(D4/J7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="K15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="L15" s="7" t="n">
+      <c r="L15" s="9" t="n">
         <f aca="false">MIN(3*(D4/L7)/D5,D6)</f>
         <v>1048575</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J22" s="9" t="s">
-        <v>26</v>
+      <c r="J22" s="10" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E29" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E30" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D32" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E32" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10" t="s">
+      <c r="E32" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H32" s="10" t="s">
+      <c r="F32" s="11"/>
+      <c r="G32" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I32" s="10" t="s">
+      <c r="H32" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J32" s="10" t="s">
+      <c r="I32" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="K32" s="10" t="s">
+      <c r="J32" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="L32" s="10" t="n">
+      <c r="K32" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L32" s="11" t="n">
         <v>96467329</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E33" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E34" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E35" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E37" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E38" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E39" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2612,58 +2653,58 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G11" s="5"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>24</v>
+      <c r="C12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D13" s="6" t="n">
+      <c r="D13" s="7" t="n">
         <f aca="false">MIN(1*(D4/D7)/D5, D6)</f>
         <v>739555.555555556</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="6" t="n">
+      <c r="F13" s="7" t="n">
         <f aca="false">MIN(1*(D4/F7)/D5, D6)</f>
         <v>633904.761904762</v>
       </c>
       <c r="G13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H13" s="7" t="n">
+      <c r="H13" s="9" t="n">
         <f aca="false">MIN((D4/H7)/D5, D6)</f>
         <v>522039.215686275</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J13" s="7" t="n">
+      <c r="J13" s="9" t="n">
         <f aca="false">MIN(1*(D4/J7)/D5, D6)</f>
         <v>467087.719298246</v>
       </c>
       <c r="K13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L13" s="7" t="n">
+      <c r="L13" s="9" t="n">
         <f aca="false">MIN(1*(D4/L7)/D5, D6)</f>
         <v>354986.666666667</v>
       </c>
@@ -2672,35 +2713,35 @@
       <c r="C14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="D14" s="9" t="n">
         <f aca="false">MIN(2*(D4/D7) / D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F14" s="7" t="n">
+      <c r="F14" s="9" t="n">
         <f aca="false">MIN(2*(D4/F7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="G14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H14" s="6" t="n">
+      <c r="H14" s="7" t="n">
         <f aca="false">MIN(2*(D4/H7)/D5, D6)</f>
         <v>1044078.43137255</v>
       </c>
       <c r="I14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="J14" s="6" t="n">
+      <c r="J14" s="7" t="n">
         <f aca="false">MIN(2*(D4/J7)/D5,D6)</f>
         <v>934175.438596491</v>
       </c>
       <c r="K14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="L14" s="6" t="n">
+      <c r="L14" s="7" t="n">
         <f aca="false">MIN(2*(D4/L7)/D5, D6)</f>
         <v>709973.333333333</v>
       </c>
@@ -2709,119 +2750,119 @@
       <c r="C15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D15" s="7" t="n">
+      <c r="D15" s="9" t="n">
         <f aca="false">MIN(3*(D4/D7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F15" s="7" t="n">
+      <c r="F15" s="9" t="n">
         <f aca="false">MIN(3*(D6/F7)/D5, D6)</f>
         <v>76695.7714285714</v>
       </c>
       <c r="G15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="H15" s="7" t="n">
+      <c r="H15" s="9" t="n">
         <f aca="false">MIN(3*(D4/H7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="I15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="J15" s="7" t="n">
+      <c r="J15" s="9" t="n">
         <f aca="false">MIN(3*(D4/J7)/D5, D6)</f>
         <v>1048575</v>
       </c>
       <c r="K15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="L15" s="7" t="n">
+      <c r="L15" s="9" t="n">
         <f aca="false">MIN(3*(D4/L7)/D5,D6)</f>
         <v>1048575</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J22" s="9" t="s">
-        <v>26</v>
+      <c r="J22" s="10" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E29" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E30" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D32" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E32" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10" t="s">
+      <c r="E32" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H32" s="10" t="s">
+      <c r="F32" s="11"/>
+      <c r="G32" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I32" s="10" t="s">
+      <c r="H32" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J32" s="10" t="s">
+      <c r="I32" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="K32" s="10" t="s">
+      <c r="J32" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="L32" s="10" t="n">
+      <c r="K32" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L32" s="11" t="n">
         <v>96467329</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E33" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E34" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E35" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E37" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E38" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E39" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>